<commit_message>
Dairy tables added in session schema xls
</commit_message>
<xml_diff>
--- a/application-service/src/test/resources/ExaminationModule_Schema.xlsx
+++ b/application-service/src/test/resources/ExaminationModule_Schema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
   <si>
     <t>Exam</t>
   </si>
@@ -232,6 +232,54 @@
   </si>
   <si>
     <t>ObtainedMarks</t>
+  </si>
+  <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>Id_Dairy</t>
+  </si>
+  <si>
+    <t>ID_SESSION</t>
+  </si>
+  <si>
+    <t>ID_SUBJECT</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Read chapter -1</t>
+  </si>
+  <si>
+    <t>Test on Tuesday</t>
+  </si>
+  <si>
+    <t>ID_SECTION</t>
+  </si>
+  <si>
+    <t>Student_Dairy</t>
+  </si>
+  <si>
+    <t>Id_StudentDairy</t>
+  </si>
+  <si>
+    <t>ID_StudentSection</t>
+  </si>
+  <si>
+    <t>AudienceID</t>
   </si>
 </sst>
 </file>
@@ -335,7 +383,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -395,15 +443,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -412,6 +477,12 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -421,12 +492,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,17 +806,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M35"/>
+  <dimension ref="B2:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
@@ -752,637 +830,786 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="J2" s="10" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="J2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="12"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="13">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="3">
-        <v>1</v>
-      </c>
-      <c r="K4" s="4" t="s">
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="13">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5">
-        <v>2</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="B5" s="9">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="4">
-        <v>2</v>
-      </c>
-      <c r="K5" s="4" t="s">
+      <c r="J5" s="3">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>3</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="12">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
         <v>0</v>
       </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="J9" s="10" t="s">
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="12"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="17"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
-        <v>2</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="12">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="9">
-        <v>2</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="D10" s="8">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3">
         <v>0</v>
       </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="2" t="s">
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J11" s="5">
-        <v>1</v>
-      </c>
-      <c r="K11" s="3">
-        <v>1</v>
-      </c>
-      <c r="L11" s="4" t="s">
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J12" s="5">
-        <v>2</v>
-      </c>
-      <c r="K12" s="3">
-        <v>1</v>
-      </c>
-      <c r="L12" s="4" t="s">
+      <c r="J12" s="4">
+        <v>2</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="J13" s="4">
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="J13" s="3">
         <v>3</v>
       </c>
-      <c r="K13" s="4">
-        <v>2</v>
-      </c>
-      <c r="L13" s="4" t="s">
+      <c r="K13" s="3">
+        <v>2</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2" t="s">
+      <c r="G14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="18">
-        <v>1</v>
-      </c>
-      <c r="C15" s="16">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="B15" s="14">
+        <v>1</v>
+      </c>
+      <c r="C15" s="12">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
         <v>25</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>12</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="13">
-        <v>1</v>
-      </c>
-      <c r="H15" s="15">
+      <c r="F15" s="10"/>
+      <c r="G15" s="9">
+        <v>1</v>
+      </c>
+      <c r="H15" s="11">
         <v>43713</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="18">
-        <v>2</v>
-      </c>
-      <c r="C16" s="16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="B16" s="14">
+        <v>2</v>
+      </c>
+      <c r="C16" s="12">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
         <v>25</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>12</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="13">
-        <v>2</v>
-      </c>
-      <c r="H16" s="15">
+      <c r="F16" s="10"/>
+      <c r="G16" s="9">
+        <v>2</v>
+      </c>
+      <c r="H16" s="11">
         <v>43713</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="12"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="J18" s="6">
-        <v>1</v>
-      </c>
-      <c r="K18" s="4" t="s">
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="J18" s="5">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="6">
         <v>43525</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="6">
         <v>43891</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J19" s="4">
-        <v>2</v>
-      </c>
-      <c r="K19" s="4" t="s">
+      <c r="J19" s="3">
+        <v>2</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="6">
         <v>43891</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="6">
         <v>44256</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="8">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="7">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20" s="15">
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="11">
         <v>43713</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="11">
         <v>43713</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="8">
-        <v>2</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="7">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="4">
-        <v>2</v>
-      </c>
-      <c r="E21" s="15">
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21" s="11">
         <v>43713</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="11">
         <v>43713</v>
       </c>
-      <c r="G21" s="6">
-        <v>1</v>
-      </c>
-      <c r="J21" s="10" t="s">
+      <c r="G21" s="5">
+        <v>1</v>
+      </c>
+      <c r="J21" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="12"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="17"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="8">
+      <c r="B22" s="7">
         <v>3</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>3</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="11">
         <v>43713</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="11">
         <v>43713</v>
       </c>
-      <c r="G22" s="6">
-        <v>1</v>
-      </c>
-      <c r="J22" s="2" t="s">
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="K22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="L22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="M22" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J23" s="9">
-        <v>1</v>
-      </c>
-      <c r="K23" s="4" t="s">
+      <c r="J23" s="8">
+        <v>1</v>
+      </c>
+      <c r="K23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="L23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="M23" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J24" s="9">
-        <v>2</v>
-      </c>
-      <c r="K24" s="4" t="s">
+      <c r="J24" s="8">
+        <v>2</v>
+      </c>
+      <c r="K24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L24" s="4" t="s">
+      <c r="L24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M24" s="4" t="s">
+      <c r="M24" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2" t="s">
+      <c r="E26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="17">
-        <v>1</v>
-      </c>
-      <c r="C27" s="8">
-        <v>1</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="B27" s="13">
+        <v>1</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="13">
-        <v>1</v>
-      </c>
-      <c r="F27" s="4" t="s">
+      <c r="E27" s="9">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="4">
-        <v>2</v>
-      </c>
-      <c r="C28" s="8">
-        <v>2</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="B28" s="3">
+        <v>2</v>
+      </c>
+      <c r="C28" s="7">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E28" s="13">
-        <v>1</v>
-      </c>
-      <c r="F28" s="4" t="s">
+      <c r="E28" s="9">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>3</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="7">
         <v>3</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E29" s="13">
-        <v>1</v>
-      </c>
-      <c r="F29" s="4" t="s">
+      <c r="E29" s="9">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-      <c r="C34" s="17">
-        <v>1</v>
-      </c>
-      <c r="D34" s="4">
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+      <c r="C34" s="13">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3">
         <v>20</v>
       </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="18">
-        <v>1</v>
-      </c>
-      <c r="G34" s="4">
-        <v>1</v>
-      </c>
-      <c r="H34" s="4">
+      <c r="E34" s="10"/>
+      <c r="F34" s="14">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3">
+        <v>1</v>
+      </c>
+      <c r="H34" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="4">
-        <v>2</v>
-      </c>
-      <c r="C35" s="17">
-        <v>1</v>
-      </c>
-      <c r="D35" s="4">
+      <c r="B35" s="3">
+        <v>2</v>
+      </c>
+      <c r="C35" s="13">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3">
         <v>18</v>
       </c>
-      <c r="E35" s="14"/>
-      <c r="F35" s="18">
-        <v>2</v>
-      </c>
-      <c r="G35" s="4">
-        <v>1</v>
-      </c>
-      <c r="H35" s="4">
-        <v>1</v>
-      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="14">
+        <v>2</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="3">
+        <v>1</v>
+      </c>
+      <c r="C40" s="8">
+        <v>1</v>
+      </c>
+      <c r="D40" s="12">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3">
+        <v>1</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G40" s="21">
+        <v>43525</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <v>2</v>
+      </c>
+      <c r="C41" s="8">
+        <v>1</v>
+      </c>
+      <c r="D41" s="12">
+        <v>2</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G41" s="21">
+        <v>43526</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="3">
+        <v>1</v>
+      </c>
+      <c r="C46" s="8">
+        <v>1</v>
+      </c>
+      <c r="D46" s="12">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="3">
+        <v>2</v>
+      </c>
+      <c r="C47" s="8">
+        <v>1</v>
+      </c>
+      <c r="D47" s="12">
+        <v>2</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="B44:E44"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="B25:F25"/>

</xml_diff>